<commit_message>
i have to test it on phone
</commit_message>
<xml_diff>
--- a/data/correlation_matrix.xlsx
+++ b/data/correlation_matrix.xlsx
@@ -533,7 +533,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AY45"/>
+  <dimension ref="A1:AS45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
@@ -543,7 +543,7 @@
   <cols>
     <col min="1" max="44" width="23.5546875" customWidth="1"/>
     <col min="45" max="45" width="18.109375" customWidth="1"/>
-    <col min="46" max="61" width="23.5546875" customWidth="1"/>
+    <col min="46" max="55" width="23.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:45" x14ac:dyDescent="0.3">
@@ -4912,7 +4912,7 @@
         <v>-0.12429704499461849</v>
       </c>
     </row>
-    <row r="33" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>28</v>
       </c>
@@ -5049,7 +5049,7 @@
         <v>-0.1069548623286298</v>
       </c>
     </row>
-    <row r="34" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>29</v>
       </c>
@@ -5186,7 +5186,7 @@
         <v>-5.5525338516318641E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>30</v>
       </c>
@@ -5323,7 +5323,7 @@
         <v>0.1998053548885334</v>
       </c>
     </row>
-    <row r="36" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>31</v>
       </c>
@@ -5459,20 +5459,8 @@
       <c r="AS36">
         <v>0.20749597526992669</v>
       </c>
-      <c r="AT36">
-        <v>-0.43671977869309281</v>
-      </c>
-      <c r="AU36">
-        <v>-3.4790534451490288E-2</v>
-      </c>
-      <c r="AV36">
-        <v>-0.57332155365683868</v>
-      </c>
-      <c r="AW36">
-        <v>-0.36432981603506498</v>
-      </c>
     </row>
-    <row r="37" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>32</v>
       </c>
@@ -5608,26 +5596,8 @@
       <c r="AS37">
         <v>0.20153378614045969</v>
       </c>
-      <c r="AT37" s="2">
-        <v>-0.52787782202226441</v>
-      </c>
-      <c r="AU37" s="2">
-        <v>5.0436556308725067E-2</v>
-      </c>
-      <c r="AV37" s="2">
-        <v>-0.59529050616902035</v>
-      </c>
-      <c r="AW37" s="2">
-        <v>-0.45696676370066508</v>
-      </c>
-      <c r="AX37" s="2">
-        <v>-0.41303908077282148</v>
-      </c>
-      <c r="AY37" s="2">
-        <v>-0.64985525003830813</v>
-      </c>
     </row>
-    <row r="38" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>33</v>
       </c>
@@ -5763,26 +5733,8 @@
       <c r="AS38">
         <v>0.187433841693039</v>
       </c>
-      <c r="AT38" s="2">
-        <v>-0.25279384489057038</v>
-      </c>
-      <c r="AU38" s="2">
-        <v>-0.85159197619698446</v>
-      </c>
-      <c r="AV38" s="2">
-        <v>-9.676970423723355E-2</v>
-      </c>
-      <c r="AW38" s="2">
-        <v>-5.0806298594445402E-2</v>
-      </c>
-      <c r="AX38" s="2">
-        <v>-0.57083442689595998</v>
-      </c>
-      <c r="AY38" s="2">
-        <v>-0.28400267664711132</v>
-      </c>
     </row>
-    <row r="39" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>34</v>
       </c>
@@ -5918,23 +5870,8 @@
       <c r="AS39">
         <v>-1.111719786997041E-2</v>
       </c>
-      <c r="AT39">
-        <v>-0.29852495298625531</v>
-      </c>
-      <c r="AU39">
-        <v>-0.40647010664887739</v>
-      </c>
-      <c r="AV39">
-        <v>-0.17141193960772341</v>
-      </c>
-      <c r="AW39">
-        <v>-0.47092287157505669</v>
-      </c>
-      <c r="AX39">
-        <v>-0.26149219464775952</v>
-      </c>
     </row>
-    <row r="40" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>35</v>
       </c>
@@ -6070,23 +6007,8 @@
       <c r="AS40">
         <v>7.6410037285390177E-3</v>
       </c>
-      <c r="AT40" s="2">
-        <v>-1.643107533584176E-2</v>
-      </c>
-      <c r="AU40" s="2">
-        <v>-0.43605416482490728</v>
-      </c>
-      <c r="AV40" s="2">
-        <v>-0.2494749645808349</v>
-      </c>
-      <c r="AW40" s="2">
-        <v>-0.32958987628786962</v>
-      </c>
-      <c r="AX40" s="2">
-        <v>-0.2576834764839997</v>
-      </c>
     </row>
-    <row r="41" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>36</v>
       </c>
@@ -6222,17 +6144,8 @@
       <c r="AS41">
         <v>-0.37074717950604003</v>
       </c>
-      <c r="AT41">
-        <v>-0.41456898861808689</v>
-      </c>
-      <c r="AU41">
-        <v>-0.40330503731250161</v>
-      </c>
-      <c r="AV41">
-        <v>-0.22044598024007311</v>
-      </c>
     </row>
-    <row r="42" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>37</v>
       </c>
@@ -6368,17 +6281,8 @@
       <c r="AS42">
         <v>0.13370748175157621</v>
       </c>
-      <c r="AT42" s="2">
-        <v>-0.62131752493062287</v>
-      </c>
-      <c r="AU42" s="2">
-        <v>-0.48106454152725259</v>
-      </c>
-      <c r="AV42" s="2">
-        <v>-0.65583930974094051</v>
-      </c>
     </row>
-    <row r="43" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>38</v>
       </c>
@@ -6514,17 +6418,8 @@
       <c r="AS43">
         <v>3.7191073203250158E-2</v>
       </c>
-      <c r="AT43" s="2">
-        <v>-0.32566059926584467</v>
-      </c>
-      <c r="AU43" s="2">
-        <v>-0.89914134046137462</v>
-      </c>
-      <c r="AV43" s="2">
-        <v>-0.2353626854766831</v>
-      </c>
     </row>
-    <row r="44" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>39</v>
       </c>
@@ -6660,17 +6555,8 @@
       <c r="AS44">
         <v>0.41198934236450568</v>
       </c>
-      <c r="AT44">
-        <v>-0.48538388817930939</v>
-      </c>
-      <c r="AU44">
-        <v>0.22963349234553079</v>
-      </c>
-      <c r="AV44">
-        <v>-0.50415312340104634</v>
-      </c>
     </row>
-    <row r="45" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>40</v>
       </c>
@@ -6805,15 +6691,6 @@
       </c>
       <c r="AS45">
         <v>1</v>
-      </c>
-      <c r="AT45">
-        <v>-0.38732646197741338</v>
-      </c>
-      <c r="AU45">
-        <v>-0.42052201627065039</v>
-      </c>
-      <c r="AV45">
-        <v>-0.65252432859925857</v>
       </c>
     </row>
   </sheetData>

</xml_diff>